<commit_message>
hopefully it should "work".. enough to make regression data at least
</commit_message>
<xml_diff>
--- a/testOpenCV/tg_r2.xlsx
+++ b/testOpenCV/tg_r2.xlsx
@@ -9,19 +9,45 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1." sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Statiske 1-5mm" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr autoRecover="0" repairLoad="1"/>
+  <pivotCaches>
+    <pivotCache cacheId="10" r:id="rId5"/>
+  </pivotCaches>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>StdDev of 5</t>
+  </si>
+  <si>
+    <t>StdDev of 4</t>
+  </si>
+  <si>
+    <t>StdDev of 3</t>
+  </si>
+  <si>
+    <t>StdDev of 2</t>
+  </si>
+  <si>
+    <t>StdDev of 1</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,9 +81,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -110,13 +138,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="da-DK"/>
-              <a:t>Linear</a:t>
+              <a:t>*Foreløbig</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="da-DK" baseline="0"/>
-              <a:t> regression (tg)</a:t>
-            </a:r>
-            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -240,7 +263,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$1:$D$3</c:f>
+              <c:f>'1.'!$D$1:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -258,7 +281,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$3</c:f>
+              <c:f>'1.'!$E$1:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -461,7 +484,626 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[tg_r2.xlsx]Sheet3!PivotTable5</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StdDev of 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$A$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.23900829627183379</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-99AF-4ABD-977A-E01DAF9EB3CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StdDev of 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.36340127664069305</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-99AF-4ABD-977A-E01DAF9EB3CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StdDev of 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.6911935205442058</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-99AF-4ABD-977A-E01DAF9EB3CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StdDev of 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.47491268068513637</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-99AF-4ABD-977A-E01DAF9EB3CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StdDev of 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.59320423040618409</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-99AF-4ABD-977A-E01DAF9EB3CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="511639896"/>
+        <c:axId val="511641536"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="511639896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="511641536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="511641536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="511639896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -998,6 +1640,509 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1056,6 +2201,248 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B522E47-A634-493E-B9F5-6395739C7403}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Rudy Alex Kohn" refreshedDate="42920.646131018519" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="10">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:E11" sheet="Statiske 1-5mm"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="1" numFmtId="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="9.1957799999999992" maxValue="9.9805969999999995"/>
+    </cacheField>
+    <cacheField name="2" numFmtId="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="15.809569" maxValue="17.085523999999999"/>
+    </cacheField>
+    <cacheField name="3" numFmtId="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="22.635497000000001" maxValue="24.485149"/>
+    </cacheField>
+    <cacheField name="4" numFmtId="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="30.122298000000001" maxValue="31.392472999999999"/>
+    </cacheField>
+    <cacheField name="5" numFmtId="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="37.921579000000001" maxValue="39.489227"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="10">
+  <r>
+    <n v="9.2969059999999999"/>
+    <n v="16.441233"/>
+    <n v="23.515231"/>
+    <n v="31.392472999999999"/>
+    <n v="38.605896999999999"/>
+  </r>
+  <r>
+    <n v="9.2290399999999995"/>
+    <n v="16.150548000000001"/>
+    <n v="24.456081999999999"/>
+    <n v="31.068819999999999"/>
+    <n v="39.166429000000001"/>
+  </r>
+  <r>
+    <n v="9.9805969999999995"/>
+    <n v="16.422732"/>
+    <n v="24.485149"/>
+    <n v="30.122298000000001"/>
+    <n v="38.496259000000002"/>
+  </r>
+  <r>
+    <n v="9.2185299999999994"/>
+    <n v="16.376899000000002"/>
+    <n v="22.827715999999999"/>
+    <n v="30.620356999999998"/>
+    <n v="38.007728999999998"/>
+  </r>
+  <r>
+    <n v="9.2144890000000004"/>
+    <n v="16.221957"/>
+    <n v="24.403165000000001"/>
+    <n v="30.362038999999999"/>
+    <n v="39.331057000000001"/>
+  </r>
+  <r>
+    <n v="9.1957799999999992"/>
+    <n v="15.809569"/>
+    <n v="24.336946000000001"/>
+    <n v="30.433250000000001"/>
+    <n v="39.166576999999997"/>
+  </r>
+  <r>
+    <n v="9.1970849999999995"/>
+    <n v="16.726089999999999"/>
+    <n v="23.396470999999998"/>
+    <n v="30.123169000000001"/>
+    <n v="39.489227"/>
+  </r>
+  <r>
+    <n v="9.3070740000000001"/>
+    <n v="16.141902000000002"/>
+    <n v="23.530507"/>
+    <n v="31.236001999999999"/>
+    <n v="37.921579000000001"/>
+  </r>
+  <r>
+    <n v="9.2109810000000003"/>
+    <n v="16.718219000000001"/>
+    <n v="22.635497000000001"/>
+    <n v="31.081012999999999"/>
+    <n v="39.371673999999999"/>
+  </r>
+  <r>
+    <n v="9.2421369999999996"/>
+    <n v="17.085523999999999"/>
+    <n v="23.295247"/>
+    <n v="31.089407999999999"/>
+    <n v="39.416347000000002"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A1:E2" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </colItems>
+  <dataFields count="5">
+    <dataField name="StdDev of 1" fld="0" subtotal="stdDev" baseField="0" baseItem="1"/>
+    <dataField name="StdDev of 2" fld="1" subtotal="stdDev" baseField="0" baseItem="1"/>
+    <dataField name="StdDev of 3" fld="2" subtotal="stdDev" baseField="0" baseItem="1"/>
+    <dataField name="StdDev of 4" fld="3" subtotal="stdDev" baseField="0" baseItem="1"/>
+    <dataField name="StdDev of 5" fld="4" subtotal="stdDev" baseField="0" baseItem="1"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1357,8 +2744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,12 +2762,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>8.5547140000000006</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="D2">
         <v>1</v>
       </c>
@@ -1389,12 +2771,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>15.863046000000001</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="D3">
         <v>2</v>
       </c>
@@ -1404,6 +2781,279 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0.23900829627183379</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.36340127664069305</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.6911935205442058</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.47491268068513637</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.59320423040618409</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>9.2969059999999999</v>
+      </c>
+      <c r="B2" s="2">
+        <v>16.441233</v>
+      </c>
+      <c r="C2" s="2">
+        <v>23.515231</v>
+      </c>
+      <c r="D2" s="2">
+        <v>31.392472999999999</v>
+      </c>
+      <c r="E2" s="2">
+        <v>38.605896999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>9.2290399999999995</v>
+      </c>
+      <c r="B3" s="2">
+        <v>16.150548000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <v>24.456081999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>31.068819999999999</v>
+      </c>
+      <c r="E3" s="2">
+        <v>39.166429000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>9.9805969999999995</v>
+      </c>
+      <c r="B4" s="2">
+        <v>16.422732</v>
+      </c>
+      <c r="C4" s="2">
+        <v>24.485149</v>
+      </c>
+      <c r="D4" s="2">
+        <v>30.122298000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>38.496259000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>9.2185299999999994</v>
+      </c>
+      <c r="B5" s="2">
+        <v>16.376899000000002</v>
+      </c>
+      <c r="C5" s="2">
+        <v>22.827715999999999</v>
+      </c>
+      <c r="D5" s="2">
+        <v>30.620356999999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>38.007728999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>9.2144890000000004</v>
+      </c>
+      <c r="B6" s="2">
+        <v>16.221957</v>
+      </c>
+      <c r="C6" s="2">
+        <v>24.403165000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>30.362038999999999</v>
+      </c>
+      <c r="E6" s="2">
+        <v>39.331057000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>9.1957799999999992</v>
+      </c>
+      <c r="B7" s="2">
+        <v>15.809569</v>
+      </c>
+      <c r="C7" s="2">
+        <v>24.336946000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>30.433250000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>39.166576999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>9.1970849999999995</v>
+      </c>
+      <c r="B8" s="2">
+        <v>16.726089999999999</v>
+      </c>
+      <c r="C8" s="2">
+        <v>23.396470999999998</v>
+      </c>
+      <c r="D8" s="2">
+        <v>30.123169000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>39.489227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>9.3070740000000001</v>
+      </c>
+      <c r="B9" s="2">
+        <v>16.141902000000002</v>
+      </c>
+      <c r="C9" s="2">
+        <v>23.530507</v>
+      </c>
+      <c r="D9" s="2">
+        <v>31.236001999999999</v>
+      </c>
+      <c r="E9" s="2">
+        <v>37.921579000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9.2109810000000003</v>
+      </c>
+      <c r="B10" s="2">
+        <v>16.718219000000001</v>
+      </c>
+      <c r="C10" s="2">
+        <v>22.635497000000001</v>
+      </c>
+      <c r="D10" s="2">
+        <v>31.081012999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <v>39.371673999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9.2421369999999996</v>
+      </c>
+      <c r="B11" s="2">
+        <v>17.085523999999999</v>
+      </c>
+      <c r="C11" s="2">
+        <v>23.295247</v>
+      </c>
+      <c r="D11" s="2">
+        <v>31.089407999999999</v>
+      </c>
+      <c r="E11" s="2">
+        <v>39.416347000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated sheet with another measurement + added images
</commit_message>
<xml_diff>
--- a/testOpenCV/tg_r2.xlsx
+++ b/testOpenCV/tg_r2.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1." sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
-    <sheet name="Statiske 1-5mm" sheetId="2" r:id="rId4"/>
+    <sheet name="2." sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="Statiske 1-5mm" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>#1</t>
   </si>
@@ -97,6 +98,18 @@
   </si>
   <si>
     <t>stddev</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>**) Mindre udsving kan forekomme, grundet lokale forstyrrelser, som f.eks. En arm placeres på bordet.</t>
+  </si>
+  <si>
+    <t>*) Målingsmetoden er ikke hjulpet af den regulære baggrund hvor laseren normalt er lokaliseret</t>
   </si>
 </sst>
 </file>
@@ -188,12 +201,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="da-DK"/>
-              <a:t>Gennemsnit</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="da-DK" baseline="0"/>
-              <a:t> af 50 målinger i hver højde</a:t>
+              <a:t>50 målinger i hver højde (071117)</a:t>
             </a:r>
             <a:endParaRPr lang="da-DK"/>
           </a:p>
@@ -203,8 +212,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20011111111111113"/>
-          <c:y val="2.7777777777777776E-2"/>
+          <c:x val="0.36456838959701743"/>
+          <c:y val="2.777771199652675E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -359,7 +368,7 @@
                 <c:pt idx="1">
                   <c:v>8.182063160000002</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
+                <c:pt idx="2">
                   <c:v>15.730937959999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
@@ -565,6 +574,412 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="da-DK" baseline="0"/>
+              <a:t>25 målinger i hver højde (071217)</a:t>
+            </a:r>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35073553740812285"/>
+          <c:y val="2.777771199652675E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.9234470691163604E-4"/>
+                  <c:y val="0.3051388888888889"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="da-DK"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2.'!$P$2:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'2.'!$Q$2:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.2187543600000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2173388400000018</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.705651960000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.036377400000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.487089279999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37.959033560000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45.635390080000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D5BF-43D4-8272-B083ACD7DEA3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="356757008"/>
+        <c:axId val="356759304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="356757008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="356759304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="356759304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="356757008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1188,7 +1603,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2437,6 +2852,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3470,7 +3925,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3497,8 +3952,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3599,6 +4054,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3977,15 +4948,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>404812</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:colOff>442912</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>100012</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4014,6 +4985,49 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D166703-5C3B-487C-BEF4-E932A7E3F486}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4056,7 +5070,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4598,10 +5612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R51"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4611,7 +5625,7 @@
     <col min="4" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -4655,7 +5669,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3.2434099999999999</v>
       </c>
@@ -4681,15 +5695,18 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <f>AVERAGE(A2:A101)</f>
+        <f>AVERAGE(A2:A51)</f>
         <v>2.9569165999999996</v>
       </c>
       <c r="R2">
-        <f>_xlfn.STDEV.P(A2:A51)</f>
-        <v>0.68003707355587895</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <f>STDEV(A2:A51)</f>
+        <v>0.68694118024230966</v>
+      </c>
+      <c r="S2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.5791599999999999</v>
       </c>
@@ -4715,15 +5732,15 @@
         <v>1</v>
       </c>
       <c r="Q3" s="1">
-        <f>AVERAGE(B2:B101)</f>
+        <f>AVERAGE(B2:B51)</f>
         <v>8.182063160000002</v>
       </c>
       <c r="R3">
-        <f>_xlfn.STDEV.P(B2:B51)</f>
-        <v>0.13256666257583152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <f>STDEV(B2:B51)</f>
+        <v>0.13391255152377057</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3.2730700000000001</v>
       </c>
@@ -4748,16 +5765,16 @@
       <c r="P4">
         <v>2</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="1">
         <f>AVERAGE(C2:C51)</f>
         <v>15.730937959999999</v>
       </c>
       <c r="R4">
-        <f>_xlfn.STDEV.P(C2:C51)</f>
-        <v>0.1097162056055459</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <f>STDEV(C2:C51)</f>
+        <v>0.1108301042710557</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2.3410000000000002</v>
       </c>
@@ -4787,11 +5804,14 @@
         <v>22.741547880000002</v>
       </c>
       <c r="R5">
-        <f>_xlfn.STDEV.P(D2:D51)</f>
-        <v>0.41057380987455289</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <f>STDEV(D2:D51)</f>
+        <v>0.41474217877127523</v>
+      </c>
+      <c r="S5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2.85602</v>
       </c>
@@ -4821,11 +5841,11 @@
         <v>30.447300559999995</v>
       </c>
       <c r="R6">
-        <f>_xlfn.STDEV.P(E2:E51)</f>
-        <v>0.11848661513473313</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <f>STDEV(E2:E51)</f>
+        <v>0.11968955577372917</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2.3264200000000002</v>
       </c>
@@ -4855,11 +5875,11 @@
         <v>37.688636120000005</v>
       </c>
       <c r="R7">
-        <f>_xlfn.STDEV.P(F2:F51)</f>
-        <v>0.12942977282953694</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <f>STDEV(F2:F51)</f>
+        <v>0.1307438143645713</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3.3054199999999998</v>
       </c>
@@ -4889,11 +5909,11 @@
         <v>45.509791020000002</v>
       </c>
       <c r="R8">
-        <f>_xlfn.STDEV.P(G2:G51)</f>
-        <v>0.12887268826209733</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <f>STDEV(G2:G51)</f>
+        <v>0.13018107397124146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3.28918</v>
       </c>
@@ -4916,7 +5936,7 @@
         <v>45.626207000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2.8544299999999998</v>
       </c>
@@ -4939,7 +5959,7 @@
         <v>45.564689000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2.8735400000000002</v>
       </c>
@@ -4962,7 +5982,7 @@
         <v>45.210921999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2.8588900000000002</v>
       </c>
@@ -4985,7 +6005,7 @@
         <v>45.570596000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3.28369</v>
       </c>
@@ -5008,7 +6028,7 @@
         <v>45.746613000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>3.27881</v>
       </c>
@@ -5031,7 +6051,7 @@
         <v>45.496529000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3.2846700000000002</v>
       </c>
@@ -5054,7 +6074,7 @@
         <v>45.542391000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2.8435700000000002</v>
       </c>
@@ -5445,7 +6465,7 @@
         <v>45.324365</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>3.4813800000000001</v>
       </c>
@@ -5468,7 +6488,7 @@
         <v>45.412962999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>3.9319500000000001</v>
       </c>
@@ -5491,7 +6511,7 @@
         <v>45.290559999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1.17804</v>
       </c>
@@ -5514,7 +6534,7 @@
         <v>45.526136999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2.8797000000000001</v>
       </c>
@@ -5537,7 +6557,7 @@
         <v>45.582956000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1.6771199999999999</v>
       </c>
@@ -5560,7 +6580,7 @@
         <v>45.575797999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3.3087800000000001</v>
       </c>
@@ -5583,7 +6603,7 @@
         <v>45.479804999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>3.4368300000000001</v>
       </c>
@@ -5605,8 +6625,11 @@
       <c r="G39" s="1">
         <v>45.475346000000002</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1.9567300000000001</v>
       </c>
@@ -5628,8 +6651,11 @@
       <c r="G40" s="1">
         <v>45.568007000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2.69</v>
       </c>
@@ -5652,7 +6678,7 @@
         <v>45.551453000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>4.0155000000000003</v>
       </c>
@@ -5675,7 +6701,7 @@
         <v>45.525787999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>3.31915</v>
       </c>
@@ -5698,7 +6724,7 @@
         <v>45.527360999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>4.0354000000000001</v>
       </c>
@@ -5721,7 +6747,7 @@
         <v>45.523848000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2.7863799999999999</v>
       </c>
@@ -5744,7 +6770,7 @@
         <v>45.410842000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>3.3969100000000001</v>
       </c>
@@ -5767,7 +6793,7 @@
         <v>45.536431999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>3.3514400000000002</v>
       </c>
@@ -5790,7 +6816,7 @@
         <v>45.567779999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>3.4115600000000001</v>
       </c>
@@ -5890,6 +6916,731 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.140625" style="1" customWidth="1"/>
+    <col min="4" max="7" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2.8401109999999998</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8.2181660000000001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>15.778724</v>
+      </c>
+      <c r="D2" s="1">
+        <v>22.984065000000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>30.541893999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>38.111460999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45.593673000000003</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>AVERAGE(A2:A26)</f>
+        <v>2.2187543600000001</v>
+      </c>
+      <c r="R2">
+        <f>STDEV(A2:A26)</f>
+        <v>0.86350034489207916</v>
+      </c>
+      <c r="S2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3.9883820000000001</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.1771969999999996</v>
+      </c>
+      <c r="C3" s="1">
+        <v>15.82423</v>
+      </c>
+      <c r="D3" s="1">
+        <v>22.869523000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>30.571663999999998</v>
+      </c>
+      <c r="F3" s="1">
+        <v>38.078166000000003</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45.769742000000001</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>AVERAGE(B2:B26)</f>
+        <v>8.2173388400000018</v>
+      </c>
+      <c r="R3">
+        <f>STDEV(B2:B26)</f>
+        <v>5.5773929179680312E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2.8324340000000001</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8.2418519999999997</v>
+      </c>
+      <c r="C4" s="1">
+        <v>15.754426</v>
+      </c>
+      <c r="D4" s="1">
+        <v>23.016411000000002</v>
+      </c>
+      <c r="E4" s="1">
+        <v>30.538568000000001</v>
+      </c>
+      <c r="F4" s="1">
+        <v>37.957056999999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>45.623527000000003</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1">
+        <f>AVERAGE(C2:C26)</f>
+        <v>15.705651960000001</v>
+      </c>
+      <c r="R4">
+        <f>STDEV(C2:C26)</f>
+        <v>0.10600112330280584</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2.5456479999999999</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8.1795799999999996</v>
+      </c>
+      <c r="C5" s="1">
+        <v>15.55864</v>
+      </c>
+      <c r="D5" s="1">
+        <v>22.993054999999998</v>
+      </c>
+      <c r="E5" s="1">
+        <v>30.544616999999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>37.517491999999997</v>
+      </c>
+      <c r="G5" s="1">
+        <v>45.214412000000003</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="1">
+        <f>AVERAGE(D2:D26)</f>
+        <v>23.036377400000003</v>
+      </c>
+      <c r="R5">
+        <f>STDEV(D2:D26)</f>
+        <v>0.14536758340926614</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1.8964300000000001</v>
+      </c>
+      <c r="B6" s="1">
+        <v>8.2509320000000006</v>
+      </c>
+      <c r="C6" s="1">
+        <v>15.740778000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>23.115186999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>30.525527</v>
+      </c>
+      <c r="F6" s="1">
+        <v>37.909025999999997</v>
+      </c>
+      <c r="G6" s="1">
+        <v>45.755054999999999</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="1">
+        <f>AVERAGE(E2:E51)</f>
+        <v>30.487089279999996</v>
+      </c>
+      <c r="R6">
+        <f>STDEV(E2:E26)</f>
+        <v>0.1104213847353706</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1.9306669999999999</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8.3240990000000004</v>
+      </c>
+      <c r="C7" s="1">
+        <v>15.646114000000001</v>
+      </c>
+      <c r="D7" s="1">
+        <v>23.052340000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>30.468779999999999</v>
+      </c>
+      <c r="F7" s="1">
+        <v>38.156939000000001</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45.400900999999998</v>
+      </c>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="1">
+        <f>AVERAGE(F2:F26)</f>
+        <v>37.959033560000002</v>
+      </c>
+      <c r="R7">
+        <f>STDEV(F2:F26)</f>
+        <v>0.16918914996833218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2.7721870000000002</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8.4217879999999994</v>
+      </c>
+      <c r="C8" s="1">
+        <v>15.634788</v>
+      </c>
+      <c r="D8" s="1">
+        <v>23.302301</v>
+      </c>
+      <c r="E8" s="1">
+        <v>30.467188</v>
+      </c>
+      <c r="F8" s="1">
+        <v>37.479694000000002</v>
+      </c>
+      <c r="G8" s="1">
+        <v>45.813971000000002</v>
+      </c>
+      <c r="P8">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>AVERAGE(G2:G31)</f>
+        <v>45.635390080000001</v>
+      </c>
+      <c r="R8">
+        <f>STDEV(G2:G26)</f>
+        <v>0.18683792387140402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2.9057330000000001</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8.1509850000000004</v>
+      </c>
+      <c r="C9" s="1">
+        <v>15.908861999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>23.162472999999999</v>
+      </c>
+      <c r="E9" s="1">
+        <v>30.352934999999999</v>
+      </c>
+      <c r="F9" s="1">
+        <v>37.930385000000001</v>
+      </c>
+      <c r="G9" s="1">
+        <v>45.804769</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.5364120000000001</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8.1996699999999993</v>
+      </c>
+      <c r="C10" s="1">
+        <v>15.875594</v>
+      </c>
+      <c r="D10" s="1">
+        <v>23.190141000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>30.409903</v>
+      </c>
+      <c r="F10" s="1">
+        <v>37.889811999999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>45.835057999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.9982200000000001</v>
+      </c>
+      <c r="B11" s="1">
+        <v>8.2011679999999991</v>
+      </c>
+      <c r="C11" s="1">
+        <v>15.807159</v>
+      </c>
+      <c r="D11" s="1">
+        <v>22.984065000000001</v>
+      </c>
+      <c r="E11" s="1">
+        <v>30.489934000000002</v>
+      </c>
+      <c r="F11" s="1">
+        <v>37.900548000000001</v>
+      </c>
+      <c r="G11" s="1">
+        <v>45.446615999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.749241</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8.2028949999999998</v>
+      </c>
+      <c r="C12" s="1">
+        <v>15.800069000000001</v>
+      </c>
+      <c r="D12" s="1">
+        <v>22.912797999999999</v>
+      </c>
+      <c r="E12" s="1">
+        <v>30.429576999999998</v>
+      </c>
+      <c r="F12" s="1">
+        <v>38.210056000000002</v>
+      </c>
+      <c r="G12" s="1">
+        <v>45.849051000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2.8275130000000002</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8.1702490000000001</v>
+      </c>
+      <c r="C13" s="1">
+        <v>15.789232999999999</v>
+      </c>
+      <c r="D13" s="1">
+        <v>23.167394000000002</v>
+      </c>
+      <c r="E13" s="1">
+        <v>30.487176999999999</v>
+      </c>
+      <c r="F13" s="1">
+        <v>37.946930000000002</v>
+      </c>
+      <c r="G13" s="1">
+        <v>45.842092999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1.3226340000000001</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8.2277280000000008</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15.789659</v>
+      </c>
+      <c r="D14" s="1">
+        <v>22.908667999999999</v>
+      </c>
+      <c r="E14" s="1">
+        <v>30.530031000000001</v>
+      </c>
+      <c r="F14" s="1">
+        <v>37.811478999999999</v>
+      </c>
+      <c r="G14" s="1">
+        <v>45.443024000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1.54545</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8.2370859999999997</v>
+      </c>
+      <c r="C15" s="1">
+        <v>15.754818999999999</v>
+      </c>
+      <c r="D15" s="1">
+        <v>23.184457999999999</v>
+      </c>
+      <c r="E15" s="1">
+        <v>30.292079999999999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>37.918551000000001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>45.463678999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.95173</v>
+      </c>
+      <c r="B16" s="1">
+        <v>8.2287289999999995</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15.624706</v>
+      </c>
+      <c r="D16" s="1">
+        <v>22.991171999999999</v>
+      </c>
+      <c r="E16" s="1">
+        <v>30.366378999999998</v>
+      </c>
+      <c r="F16" s="1">
+        <v>37.976894000000001</v>
+      </c>
+      <c r="G16" s="1">
+        <v>45.698956000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.98347300000000004</v>
+      </c>
+      <c r="B17" s="1">
+        <v>8.134976</v>
+      </c>
+      <c r="C17" s="1">
+        <v>15.678658</v>
+      </c>
+      <c r="D17" s="1">
+        <v>23.249084</v>
+      </c>
+      <c r="E17" s="1">
+        <v>30.131889999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>38.114376</v>
+      </c>
+      <c r="G17" s="1">
+        <v>45.473585</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>2.7408800000000002</v>
+      </c>
+      <c r="B18" s="1">
+        <v>8.1995310000000003</v>
+      </c>
+      <c r="C18" s="1">
+        <v>15.639167</v>
+      </c>
+      <c r="D18" s="1">
+        <v>23.050329000000001</v>
+      </c>
+      <c r="E18" s="1">
+        <v>30.505979</v>
+      </c>
+      <c r="F18" s="1">
+        <v>37.992153000000002</v>
+      </c>
+      <c r="G18" s="1">
+        <v>45.304954000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>3.9572910000000001</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8.1902220000000003</v>
+      </c>
+      <c r="C19" s="1">
+        <v>15.752895000000001</v>
+      </c>
+      <c r="D19" s="1">
+        <v>23.212696999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>30.514828000000001</v>
+      </c>
+      <c r="F19" s="1">
+        <v>38.117981</v>
+      </c>
+      <c r="G19" s="1">
+        <v>45.430436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1.5161020000000001</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8.2036879999999996</v>
+      </c>
+      <c r="C20" s="1">
+        <v>15.540959000000001</v>
+      </c>
+      <c r="D20" s="1">
+        <v>22.897677000000002</v>
+      </c>
+      <c r="E20" s="1">
+        <v>30.556992999999999</v>
+      </c>
+      <c r="F20" s="1">
+        <v>37.905152000000001</v>
+      </c>
+      <c r="G20" s="1">
+        <v>45.679588000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1.5274449999999999</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8.2028060000000007</v>
+      </c>
+      <c r="C21" s="1">
+        <v>15.663026</v>
+      </c>
+      <c r="D21" s="1">
+        <v>22.975595999999999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>30.588861999999999</v>
+      </c>
+      <c r="F21" s="1">
+        <v>38.049903</v>
+      </c>
+      <c r="G21" s="1">
+        <v>45.851165999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>1.5255609999999999</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8.2160469999999997</v>
+      </c>
+      <c r="C22" s="1">
+        <v>15.709089000000001</v>
+      </c>
+      <c r="D22" s="1">
+        <v>22.714199000000001</v>
+      </c>
+      <c r="E22" s="1">
+        <v>30.556753</v>
+      </c>
+      <c r="F22" s="1">
+        <v>38.057431000000001</v>
+      </c>
+      <c r="G22" s="1">
+        <v>45.686298000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>3.0213489999999998</v>
+      </c>
+      <c r="B23" s="1">
+        <v>8.2080169999999999</v>
+      </c>
+      <c r="C23" s="1">
+        <v>15.533906999999999</v>
+      </c>
+      <c r="D23" s="1">
+        <v>22.852091000000001</v>
+      </c>
+      <c r="E23" s="1">
+        <v>30.626076999999999</v>
+      </c>
+      <c r="F23" s="1">
+        <v>38.006081000000002</v>
+      </c>
+      <c r="G23" s="1">
+        <v>45.660473000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>3.066287</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8.2149979999999996</v>
+      </c>
+      <c r="C24" s="1">
+        <v>15.695615999999999</v>
+      </c>
+      <c r="D24" s="1">
+        <v>23.212513000000001</v>
+      </c>
+      <c r="E24" s="1">
+        <v>30.589756999999999</v>
+      </c>
+      <c r="F24" s="1">
+        <v>37.888452999999998</v>
+      </c>
+      <c r="G24" s="1">
+        <v>45.747912999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0.55122199999999999</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8.2027099999999997</v>
+      </c>
+      <c r="C25" s="1">
+        <v>15.596434</v>
+      </c>
+      <c r="D25" s="1">
+        <v>22.976042</v>
+      </c>
+      <c r="E25" s="1">
+        <v>30.479143000000001</v>
+      </c>
+      <c r="F25" s="1">
+        <v>38.029640999999998</v>
+      </c>
+      <c r="G25" s="1">
+        <v>45.815961000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1.9364570000000001</v>
+      </c>
+      <c r="B26" s="1">
+        <v>8.2283519999999992</v>
+      </c>
+      <c r="C26" s="1">
+        <v>15.543747</v>
+      </c>
+      <c r="D26" s="1">
+        <v>22.935155999999999</v>
+      </c>
+      <c r="E26" s="1">
+        <v>30.610696000000001</v>
+      </c>
+      <c r="F26" s="1">
+        <v>38.020178000000001</v>
+      </c>
+      <c r="G26" s="1">
+        <v>45.679850999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX38"/>
   <sheetViews>
@@ -6314,7 +8065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -6367,7 +8118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U13"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated sheet + fixes for tclap bleblbeblebl
</commit_message>
<xml_diff>
--- a/testOpenCV/tg_r2.xlsx
+++ b/testOpenCV/tg_r2.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="1." sheetId="1" r:id="rId1"/>
-    <sheet name="2." sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="2" sheetId="6" r:id="rId2"/>
+    <sheet name="2b" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
     <sheet name="Statiske 1-5mm" sheetId="2" r:id="rId5"/>
   </sheets>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>#1</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Avg</t>
   </si>
   <si>
-    <t>Højde i mm</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>*) Målingsmetoden er ikke hjulpet af den regulære baggrund hvor laseren normalt er lokaliseret</t>
+  </si>
+  <si>
+    <t>*) Nulværdier er baseret på basis af samme keramikoverflade hvor stripehøjden er målt</t>
   </si>
 </sst>
 </file>
@@ -328,7 +328,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'1.'!$P$2:$P$8</c:f>
+              <c:f>'1'!$P$2:$P$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -358,7 +358,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1.'!$Q$2:$Q$8</c:f>
+              <c:f>'1'!$Q$2:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -734,7 +734,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'2.'!$P$2:$P$8</c:f>
+              <c:f>'2'!$P$2:$P$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -764,7 +764,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2.'!$Q$2:$Q$8</c:f>
+              <c:f>'2'!$Q$2:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -994,6 +994,40 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="da-DK" baseline="0"/>
+              <a:t>25 målinger i hver højde (071217) *</a:t>
+            </a:r>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35073553740812285"/>
+          <c:y val="2.777771199652675E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1006,7 +1040,7 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr algn="ctr">
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -1032,11 +1066,8 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Statiske målinger</c:v>
-          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1073,8 +1104,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.32885017497812774"/>
-                  <c:y val="-3.2824074074074075E-2"/>
+                  <c:x val="9.9234470691163604E-4"/>
+                  <c:y val="0.3051388888888889"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1107,161 +1138,62 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2b'!$P$2:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Sheet4!$B$4:$K$4,Sheet4!$B$5:$K$5,Sheet4!$B$6:$K$6,Sheet4!$B$7:$K$7,Sheet4!$B$8:$K$8)</c:f>
+              <c:f>'2b'!$Q$2:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9.2969059999999999</c:v>
+                  <c:v>0.69932027999999979</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.2290399999999995</c:v>
+                  <c:v>8.2173388400000018</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9805969999999995</c:v>
+                  <c:v>15.705651960000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2185299999999994</c:v>
+                  <c:v>23.036377400000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2144890000000004</c:v>
+                  <c:v>30.487089279999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.1957799999999992</c:v>
+                  <c:v>37.959033560000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.1970849999999995</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.3070740000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.2109810000000003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.2421369999999996</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16.441233</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>16.150548000000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16.422732</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16.376899000000002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16.221957</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15.809569</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16.726089999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>16.141902000000002</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>16.718219000000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>17.085523999999999</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>23.515231</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>24.456081999999999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>24.485149</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>22.827715999999999</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24.403165000000001</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>24.336946000000001</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>23.396470999999998</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>23.530507</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>22.635497000000001</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>23.295247</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31.392472999999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>31.068819999999999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>30.122298000000001</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>30.620356999999998</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>30.362038999999999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>30.433250000000001</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>30.123169000000001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>31.236001999999999</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>31.081012999999999</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>31.089407999999999</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>38.605896999999999</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>39.166429000000001</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>38.496259000000002</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>38.007728999999998</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>39.331057000000001</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>39.166576999999997</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>39.489227</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>37.921579000000001</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>39.371673999999999</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>39.416347000000002</c:v>
+                  <c:v>45.635390080000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1269,7 +1201,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-55EA-4FA1-9BC0-6A91C9C68944}"/>
+              <c16:uniqueId val="{00000001-D72E-4818-A030-0FDC6017E34E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1281,77 +1213,32 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="483420472"/>
-        <c:axId val="483424736"/>
+        <c:axId val="356757008"/>
+        <c:axId val="356759304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="483420472"/>
+        <c:axId val="356757008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="da-DK"/>
-                  <a:t>Antal</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="da-DK" baseline="0"/>
-                  <a:t> målinger</a:t>
-                </a:r>
-                <a:endParaRPr lang="da-DK"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
+        <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="da-DK"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="out"/>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1387,12 +1274,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483424736"/>
+        <c:crossAx val="356759304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="483424736"/>
+        <c:axId val="356759304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1412,82 +1299,8 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="da-DK"/>
-                  <a:t>Højde</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="da-DK" baseline="0"/>
-                  <a:t> i px</a:t>
-                </a:r>
-                <a:endParaRPr lang="da-DK"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="da-DK"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1523,7 +1336,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483420472"/>
+        <c:crossAx val="356757008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1535,37 +1348,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4947,15 +4729,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>442912</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>461962</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4988,16 +4770,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5031,23 +4813,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>552449</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B085302B-0C73-4260-BE01-879F02F635FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A37665A-9186-4AF8-A007-767DDB98245A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5612,10 +5394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Y39" sqref="Y39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5647,26 +5429,14 @@
       <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
       <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -5703,7 +5473,7 @@
         <v>0.68694118024230966</v>
       </c>
       <c r="S2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -5808,7 +5578,7 @@
         <v>0.41474217877127523</v>
       </c>
       <c r="S5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -6097,7 +5867,7 @@
         <v>45.521802000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2.8740800000000002</v>
       </c>
@@ -6120,7 +5890,7 @@
         <v>45.455635999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2.8660299999999999</v>
       </c>
@@ -6143,7 +5913,7 @@
         <v>45.324975999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1.8220799999999999</v>
       </c>
@@ -6166,7 +5936,7 @@
         <v>45.488613999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1.94232</v>
       </c>
@@ -6189,7 +5959,7 @@
         <v>45.537799999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3.6547900000000002</v>
       </c>
@@ -6212,7 +5982,7 @@
         <v>45.575493999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>3.2837499999999999</v>
       </c>
@@ -6235,7 +6005,7 @@
         <v>45.578932000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2.8456399999999999</v>
       </c>
@@ -6258,7 +6028,7 @@
         <v>45.597287000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>3.2759399999999999</v>
       </c>
@@ -6281,7 +6051,7 @@
         <v>45.374195999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1.94452</v>
       </c>
@@ -6304,7 +6074,7 @@
         <v>45.599074999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1.9436599999999999</v>
       </c>
@@ -6327,7 +6097,7 @@
         <v>45.494526999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3.20825</v>
       </c>
@@ -6350,7 +6120,7 @@
         <v>45.647556999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>3.2975500000000002</v>
       </c>
@@ -6373,7 +6143,7 @@
         <v>45.512618000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>3.26227</v>
       </c>
@@ -6395,8 +6165,11 @@
       <c r="G29" s="1">
         <v>45.256993000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="T29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>3.3375900000000001</v>
       </c>
@@ -6418,8 +6191,11 @@
       <c r="G30" s="1">
         <v>45.668573000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="T30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>3.3317299999999999</v>
       </c>
@@ -6442,7 +6218,7 @@
         <v>45.638264999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>3.3729200000000001</v>
       </c>
@@ -6465,7 +6241,7 @@
         <v>45.324365</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>3.4813800000000001</v>
       </c>
@@ -6488,7 +6264,7 @@
         <v>45.412962999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>3.9319500000000001</v>
       </c>
@@ -6511,7 +6287,7 @@
         <v>45.290559999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1.17804</v>
       </c>
@@ -6534,7 +6310,7 @@
         <v>45.526136999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2.8797000000000001</v>
       </c>
@@ -6557,7 +6333,7 @@
         <v>45.582956000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1.6771199999999999</v>
       </c>
@@ -6580,7 +6356,7 @@
         <v>45.575797999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3.3087800000000001</v>
       </c>
@@ -6603,7 +6379,7 @@
         <v>45.479804999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>3.4368300000000001</v>
       </c>
@@ -6625,11 +6401,8 @@
       <c r="G39" s="1">
         <v>45.475346000000002</v>
       </c>
-      <c r="I39" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1.9567300000000001</v>
       </c>
@@ -6651,11 +6424,8 @@
       <c r="G40" s="1">
         <v>45.568007000000001</v>
       </c>
-      <c r="I40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2.69</v>
       </c>
@@ -6678,7 +6448,7 @@
         <v>45.551453000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>4.0155000000000003</v>
       </c>
@@ -6701,7 +6471,7 @@
         <v>45.525787999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>3.31915</v>
       </c>
@@ -6724,7 +6494,7 @@
         <v>45.527360999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>4.0354000000000001</v>
       </c>
@@ -6747,7 +6517,7 @@
         <v>45.523848000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2.7863799999999999</v>
       </c>
@@ -6770,7 +6540,7 @@
         <v>45.410842000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>3.3969100000000001</v>
       </c>
@@ -6793,7 +6563,7 @@
         <v>45.536431999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>3.3514400000000002</v>
       </c>
@@ -6816,7 +6586,7 @@
         <v>45.567779999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>3.4115600000000001</v>
       </c>
@@ -6917,10 +6687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6965,13 +6735,13 @@
         <v>10</v>
       </c>
       <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -7008,7 +6778,7 @@
         <v>0.86350034489207916</v>
       </c>
       <c r="S2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -7399,7 +7169,7 @@
         <v>45.698956000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0.98347300000000004</v>
       </c>
@@ -7422,7 +7192,7 @@
         <v>45.473585</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2.7408800000000002</v>
       </c>
@@ -7445,7 +7215,7 @@
         <v>45.304954000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>3.9572910000000001</v>
       </c>
@@ -7468,7 +7238,7 @@
         <v>45.430436</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1.5161020000000001</v>
       </c>
@@ -7491,7 +7261,7 @@
         <v>45.679588000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1.5274449999999999</v>
       </c>
@@ -7514,7 +7284,7 @@
         <v>45.851165999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1.5255609999999999</v>
       </c>
@@ -7537,7 +7307,7 @@
         <v>45.686298000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3.0213489999999998</v>
       </c>
@@ -7560,7 +7330,7 @@
         <v>45.660473000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>3.066287</v>
       </c>
@@ -7583,7 +7353,7 @@
         <v>45.747912999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>0.55122199999999999</v>
       </c>
@@ -7606,7 +7376,7 @@
         <v>45.815961000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1.9364570000000001</v>
       </c>
@@ -7629,9 +7399,9 @@
         <v>45.679850999999999</v>
       </c>
     </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I39" t="s">
-        <v>25</v>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T29" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -7642,421 +7412,722 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX38"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10.140625" style="1" customWidth="1"/>
+    <col min="4" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
-      <c r="AX1" s="1"/>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
         <v>1</v>
       </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0.673786</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8.2181660000000001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>15.778724</v>
+      </c>
+      <c r="D2" s="1">
+        <v>22.984065000000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>30.541893999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>38.111460999999998</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45.593673000000003</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>AVERAGE(A2:A26)</f>
+        <v>0.69932027999999979</v>
+      </c>
+      <c r="R2">
+        <f>STDEV(A2:A26)</f>
+        <v>1.5834934350248079E-2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.67620000000000002</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.1771969999999996</v>
+      </c>
+      <c r="C3" s="1">
+        <v>15.82423</v>
+      </c>
+      <c r="D3" s="1">
+        <v>22.869523000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>30.571663999999998</v>
+      </c>
+      <c r="F3" s="1">
+        <v>38.078166000000003</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45.769742000000001</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>AVERAGE(B2:B26)</f>
+        <v>8.2173388400000018</v>
+      </c>
+      <c r="R3">
+        <f>STDEV(B2:B26)</f>
+        <v>5.5773929179680312E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.68326100000000001</v>
+      </c>
       <c r="B4" s="1">
-        <v>9.2969059999999999</v>
+        <v>8.2418519999999997</v>
       </c>
       <c r="C4" s="1">
-        <v>9.2290399999999995</v>
+        <v>15.754426</v>
       </c>
       <c r="D4" s="1">
-        <v>9.9805969999999995</v>
+        <v>23.016411000000002</v>
       </c>
       <c r="E4" s="1">
-        <v>9.2185299999999994</v>
+        <v>30.538568000000001</v>
       </c>
       <c r="F4" s="1">
-        <v>9.2144890000000004</v>
+        <v>37.957056999999999</v>
       </c>
       <c r="G4" s="1">
-        <v>9.1957799999999992</v>
-      </c>
-      <c r="H4" s="1">
-        <v>9.1970849999999995</v>
-      </c>
-      <c r="I4" s="1">
-        <v>9.3070740000000001</v>
-      </c>
-      <c r="J4" s="1">
-        <v>9.2109810000000003</v>
-      </c>
-      <c r="K4" s="1">
-        <v>9.2421369999999996</v>
-      </c>
-      <c r="M4" s="1">
-        <f>SUM(B4:L4)</f>
-        <v>93.092618999999999</v>
-      </c>
-      <c r="N4" s="1">
-        <f>AVERAGE(B4:K4)</f>
-        <v>9.3092618999999992</v>
-      </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A5">
+        <v>45.623527000000003</v>
+      </c>
+      <c r="P4">
         <v>2</v>
       </c>
+      <c r="Q4" s="1">
+        <f>AVERAGE(C2:C26)</f>
+        <v>15.705651960000001</v>
+      </c>
+      <c r="R4">
+        <f>STDEV(C2:C26)</f>
+        <v>0.10600112330280584</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.68067800000000001</v>
+      </c>
       <c r="B5" s="1">
-        <v>16.441233</v>
+        <v>8.1795799999999996</v>
       </c>
       <c r="C5" s="1">
-        <v>16.150548000000001</v>
+        <v>15.55864</v>
       </c>
       <c r="D5" s="1">
-        <v>16.422732</v>
+        <v>22.993054999999998</v>
       </c>
       <c r="E5" s="1">
-        <v>16.376899000000002</v>
+        <v>30.544616999999999</v>
       </c>
       <c r="F5" s="1">
-        <v>16.221957</v>
+        <v>37.517491999999997</v>
       </c>
       <c r="G5" s="1">
-        <v>15.809569</v>
-      </c>
-      <c r="H5" s="1">
-        <v>16.726089999999999</v>
-      </c>
-      <c r="I5" s="1">
-        <v>16.141902000000002</v>
-      </c>
-      <c r="J5" s="1">
-        <v>16.718219000000001</v>
-      </c>
-      <c r="K5" s="1">
-        <v>17.085523999999999</v>
-      </c>
-      <c r="M5" s="1">
-        <f t="shared" ref="M5:M8" si="0">SUM(B5:L5)</f>
-        <v>164.094673</v>
-      </c>
-      <c r="N5" s="1">
-        <f t="shared" ref="N5:N8" si="1">AVERAGE(B5:K5)</f>
-        <v>16.409467299999999</v>
-      </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A6">
+        <v>45.214412000000003</v>
+      </c>
+      <c r="P5">
         <v>3</v>
       </c>
+      <c r="Q5" s="1">
+        <f>AVERAGE(D2:D26)</f>
+        <v>23.036377400000003</v>
+      </c>
+      <c r="R5">
+        <f>STDEV(D2:D26)</f>
+        <v>0.14536758340926614</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.67816100000000001</v>
+      </c>
       <c r="B6" s="1">
-        <v>23.515231</v>
+        <v>8.2509320000000006</v>
       </c>
       <c r="C6" s="1">
-        <v>24.456081999999999</v>
+        <v>15.740778000000001</v>
       </c>
       <c r="D6" s="1">
-        <v>24.485149</v>
+        <v>23.115186999999999</v>
       </c>
       <c r="E6" s="1">
-        <v>22.827715999999999</v>
+        <v>30.525527</v>
       </c>
       <c r="F6" s="1">
-        <v>24.403165000000001</v>
+        <v>37.909025999999997</v>
       </c>
       <c r="G6" s="1">
-        <v>24.336946000000001</v>
-      </c>
-      <c r="H6" s="1">
-        <v>23.396470999999998</v>
-      </c>
-      <c r="I6" s="1">
-        <v>23.530507</v>
-      </c>
-      <c r="J6" s="1">
-        <v>22.635497000000001</v>
-      </c>
-      <c r="K6" s="1">
-        <v>23.295247</v>
-      </c>
-      <c r="M6" s="1">
-        <f t="shared" si="0"/>
-        <v>236.88201099999995</v>
-      </c>
-      <c r="N6" s="1">
-        <f t="shared" si="1"/>
-        <v>23.688201099999993</v>
-      </c>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7">
+        <v>45.755054999999999</v>
+      </c>
+      <c r="P6">
         <v>4</v>
       </c>
+      <c r="Q6" s="1">
+        <f>AVERAGE(E2:E51)</f>
+        <v>30.487089279999996</v>
+      </c>
+      <c r="R6">
+        <f>STDEV(E2:E26)</f>
+        <v>0.1104213847353706</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.67172600000000005</v>
+      </c>
       <c r="B7" s="1">
-        <v>31.392472999999999</v>
+        <v>8.3240990000000004</v>
       </c>
       <c r="C7" s="1">
-        <v>31.068819999999999</v>
+        <v>15.646114000000001</v>
       </c>
       <c r="D7" s="1">
-        <v>30.122298000000001</v>
+        <v>23.052340000000001</v>
       </c>
       <c r="E7" s="1">
-        <v>30.620356999999998</v>
+        <v>30.468779999999999</v>
       </c>
       <c r="F7" s="1">
-        <v>30.362038999999999</v>
+        <v>38.156939000000001</v>
       </c>
       <c r="G7" s="1">
-        <v>30.433250000000001</v>
-      </c>
-      <c r="H7" s="1">
-        <v>30.123169000000001</v>
-      </c>
-      <c r="I7" s="1">
-        <v>31.236001999999999</v>
-      </c>
-      <c r="J7" s="1">
-        <v>31.081012999999999</v>
-      </c>
-      <c r="K7" s="1">
-        <v>31.089407999999999</v>
-      </c>
-      <c r="M7" s="1">
-        <f t="shared" si="0"/>
-        <v>307.52882899999997</v>
-      </c>
-      <c r="N7" s="1">
-        <f t="shared" si="1"/>
-        <v>30.752882899999996</v>
-      </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A8">
+        <v>45.400900999999998</v>
+      </c>
+      <c r="P7">
         <v>5</v>
       </c>
+      <c r="Q7" s="1">
+        <f>AVERAGE(F2:F26)</f>
+        <v>37.959033560000002</v>
+      </c>
+      <c r="R7">
+        <f>STDEV(F2:F26)</f>
+        <v>0.16918914996833218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.68722300000000003</v>
+      </c>
       <c r="B8" s="1">
-        <v>38.605896999999999</v>
+        <v>8.4217879999999994</v>
       </c>
       <c r="C8" s="1">
-        <v>39.166429000000001</v>
+        <v>15.634788</v>
       </c>
       <c r="D8" s="1">
-        <v>38.496259000000002</v>
+        <v>23.302301</v>
       </c>
       <c r="E8" s="1">
-        <v>38.007728999999998</v>
+        <v>30.467188</v>
       </c>
       <c r="F8" s="1">
-        <v>39.331057000000001</v>
+        <v>37.479694000000002</v>
       </c>
       <c r="G8" s="1">
-        <v>39.166576999999997</v>
-      </c>
-      <c r="H8" s="1">
-        <v>39.489227</v>
-      </c>
-      <c r="I8" s="1">
-        <v>37.921579000000001</v>
-      </c>
-      <c r="J8" s="1">
-        <v>39.371673999999999</v>
-      </c>
-      <c r="K8" s="1">
-        <v>39.416347000000002</v>
-      </c>
-      <c r="M8" s="1">
-        <f t="shared" si="0"/>
-        <v>388.97277499999996</v>
-      </c>
-      <c r="N8" s="1">
-        <f t="shared" si="1"/>
-        <v>38.897277499999994</v>
-      </c>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+        <v>45.813971000000002</v>
+      </c>
+      <c r="P8">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>AVERAGE(G2:G31)</f>
+        <v>45.635390080000001</v>
+      </c>
+      <c r="R8">
+        <f>STDEV(G2:G26)</f>
+        <v>0.18683792387140402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.69220700000000002</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8.1509850000000004</v>
+      </c>
+      <c r="C9" s="1">
+        <v>15.908861999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>23.162472999999999</v>
+      </c>
+      <c r="E9" s="1">
+        <v>30.352934999999999</v>
+      </c>
+      <c r="F9" s="1">
+        <v>37.930385000000001</v>
+      </c>
+      <c r="G9" s="1">
+        <v>45.804769</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.69850999999999996</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8.1996699999999993</v>
+      </c>
+      <c r="C10" s="1">
+        <v>15.875594</v>
+      </c>
+      <c r="D10" s="1">
+        <v>23.190141000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>30.409903</v>
+      </c>
+      <c r="F10" s="1">
+        <v>37.889811999999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>45.835057999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>0.69274899999999995</v>
+      </c>
+      <c r="B11" s="1">
+        <v>8.2011679999999991</v>
+      </c>
+      <c r="C11" s="1">
+        <v>15.807159</v>
+      </c>
+      <c r="D11" s="1">
+        <v>22.984065000000001</v>
+      </c>
+      <c r="E11" s="1">
+        <v>30.489934000000002</v>
+      </c>
+      <c r="F11" s="1">
+        <v>37.900548000000001</v>
+      </c>
+      <c r="G11" s="1">
+        <v>45.446615999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0.69511500000000004</v>
+      </c>
+      <c r="B12" s="1">
+        <v>8.2028949999999998</v>
+      </c>
+      <c r="C12" s="1">
+        <v>15.800069000000001</v>
+      </c>
+      <c r="D12" s="1">
+        <v>22.912797999999999</v>
+      </c>
+      <c r="E12" s="1">
+        <v>30.429576999999998</v>
+      </c>
+      <c r="F12" s="1">
+        <v>38.210056000000002</v>
+      </c>
+      <c r="G12" s="1">
+        <v>45.849051000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>0.70209100000000002</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8.1702490000000001</v>
+      </c>
+      <c r="C13" s="1">
+        <v>15.789232999999999</v>
+      </c>
+      <c r="D13" s="1">
+        <v>23.167394000000002</v>
+      </c>
+      <c r="E13" s="1">
+        <v>30.487176999999999</v>
+      </c>
+      <c r="F13" s="1">
+        <v>37.946930000000002</v>
+      </c>
+      <c r="G13" s="1">
+        <v>45.842092999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0.70241100000000001</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8.2277280000000008</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15.789659</v>
+      </c>
+      <c r="D14" s="1">
+        <v>22.908667999999999</v>
+      </c>
+      <c r="E14" s="1">
+        <v>30.530031000000001</v>
+      </c>
+      <c r="F14" s="1">
+        <v>37.811478999999999</v>
+      </c>
+      <c r="G14" s="1">
+        <v>45.443024000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0.71365599999999996</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8.2370859999999997</v>
+      </c>
+      <c r="C15" s="1">
+        <v>15.754818999999999</v>
+      </c>
+      <c r="D15" s="1">
+        <v>23.184457999999999</v>
+      </c>
+      <c r="E15" s="1">
+        <v>30.292079999999999</v>
+      </c>
+      <c r="F15" s="1">
+        <v>37.918551000000001</v>
+      </c>
+      <c r="G15" s="1">
+        <v>45.463678999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0.70660400000000001</v>
+      </c>
+      <c r="B16" s="1">
+        <v>8.2287289999999995</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15.624706</v>
+      </c>
+      <c r="D16" s="1">
+        <v>22.991171999999999</v>
+      </c>
+      <c r="E16" s="1">
+        <v>30.366378999999998</v>
+      </c>
+      <c r="F16" s="1">
+        <v>37.976894000000001</v>
+      </c>
+      <c r="G16" s="1">
+        <v>45.698956000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0.70759499999999997</v>
+      </c>
+      <c r="B17" s="1">
+        <v>8.134976</v>
+      </c>
+      <c r="C17" s="1">
+        <v>15.678658</v>
+      </c>
+      <c r="D17" s="1">
+        <v>23.249084</v>
+      </c>
+      <c r="E17" s="1">
+        <v>30.131889999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>38.114376</v>
+      </c>
+      <c r="G17" s="1">
+        <v>45.473585</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0.706596</v>
+      </c>
+      <c r="B18" s="1">
+        <v>8.1995310000000003</v>
+      </c>
+      <c r="C18" s="1">
+        <v>15.639167</v>
+      </c>
+      <c r="D18" s="1">
+        <v>23.050329000000001</v>
+      </c>
+      <c r="E18" s="1">
+        <v>30.505979</v>
+      </c>
+      <c r="F18" s="1">
+        <v>37.992153000000002</v>
+      </c>
+      <c r="G18" s="1">
+        <v>45.304954000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0.69668300000000005</v>
+      </c>
+      <c r="B19" s="1">
+        <v>8.1902220000000003</v>
+      </c>
+      <c r="C19" s="1">
+        <v>15.752895000000001</v>
+      </c>
+      <c r="D19" s="1">
+        <v>23.212696999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>30.514828000000001</v>
+      </c>
+      <c r="F19" s="1">
+        <v>38.117981</v>
+      </c>
+      <c r="G19" s="1">
+        <v>45.430436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.70611400000000002</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8.2036879999999996</v>
+      </c>
+      <c r="C20" s="1">
+        <v>15.540959000000001</v>
+      </c>
+      <c r="D20" s="1">
+        <v>22.897677000000002</v>
+      </c>
+      <c r="E20" s="1">
+        <v>30.556992999999999</v>
+      </c>
+      <c r="F20" s="1">
+        <v>37.905152000000001</v>
+      </c>
+      <c r="G20" s="1">
+        <v>45.679588000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>0.72446900000000003</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8.2028060000000007</v>
+      </c>
+      <c r="C21" s="1">
+        <v>15.663026</v>
+      </c>
+      <c r="D21" s="1">
+        <v>22.975595999999999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>30.588861999999999</v>
+      </c>
+      <c r="F21" s="1">
+        <v>38.049903</v>
+      </c>
+      <c r="G21" s="1">
+        <v>45.851165999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>0.71825000000000006</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8.2160469999999997</v>
+      </c>
+      <c r="C22" s="1">
+        <v>15.709089000000001</v>
+      </c>
+      <c r="D22" s="1">
+        <v>22.714199000000001</v>
+      </c>
+      <c r="E22" s="1">
+        <v>30.556753</v>
+      </c>
+      <c r="F22" s="1">
+        <v>38.057431000000001</v>
+      </c>
+      <c r="G22" s="1">
+        <v>45.686298000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>0.72056600000000004</v>
+      </c>
+      <c r="B23" s="1">
+        <v>8.2080169999999999</v>
+      </c>
+      <c r="C23" s="1">
+        <v>15.533906999999999</v>
+      </c>
+      <c r="D23" s="1">
+        <v>22.852091000000001</v>
+      </c>
+      <c r="E23" s="1">
+        <v>30.626076999999999</v>
+      </c>
+      <c r="F23" s="1">
+        <v>38.006081000000002</v>
+      </c>
+      <c r="G23" s="1">
+        <v>45.660473000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>0.71509599999999995</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8.2149979999999996</v>
+      </c>
+      <c r="C24" s="1">
+        <v>15.695615999999999</v>
+      </c>
+      <c r="D24" s="1">
+        <v>23.212513000000001</v>
+      </c>
+      <c r="E24" s="1">
+        <v>30.589756999999999</v>
+      </c>
+      <c r="F24" s="1">
+        <v>37.888452999999998</v>
+      </c>
+      <c r="G24" s="1">
+        <v>45.747912999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0.71365800000000001</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8.2027099999999997</v>
+      </c>
+      <c r="C25" s="1">
+        <v>15.596434</v>
+      </c>
+      <c r="D25" s="1">
+        <v>22.976042</v>
+      </c>
+      <c r="E25" s="1">
+        <v>30.479143000000001</v>
+      </c>
+      <c r="F25" s="1">
+        <v>38.029640999999998</v>
+      </c>
+      <c r="G25" s="1">
+        <v>45.815961000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>0.71960199999999996</v>
+      </c>
+      <c r="B26" s="1">
+        <v>8.2283519999999992</v>
+      </c>
+      <c r="C26" s="1">
+        <v>15.543747</v>
+      </c>
+      <c r="D26" s="1">
+        <v>22.935155999999999</v>
+      </c>
+      <c r="E26" s="1">
+        <v>30.610696000000001</v>
+      </c>
+      <c r="F26" s="1">
+        <v>38.020178000000001</v>
+      </c>
+      <c r="G26" s="1">
+        <v>45.679850999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T29" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8604,7 +8675,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J12" s="1">
         <v>30.393844000000001</v>

</xml_diff>

<commit_message>
Added doc to most calc:: functions
</commit_message>
<xml_diff>
--- a/testOpenCV/tg_r2.xlsx
+++ b/testOpenCV/tg_r2.xlsx
@@ -113,7 +113,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="56">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -7329,8 +7341,8 @@
   <autoFilter ref="I1:K8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="mm"/>
-    <tableColumn id="2" name="avg" dataDxfId="39"/>
-    <tableColumn id="3" name="stddev" dataDxfId="38"/>
+    <tableColumn id="2" name="avg" dataDxfId="43"/>
+    <tableColumn id="3" name="stddev" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7338,6 +7350,156 @@
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="M1:N8" totalsRowShown="0">
+  <autoFilter ref="M1:N8"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="px2mm" dataDxfId="49">
+      <calculatedColumnFormula>(J2-$J$11)/$I$11</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="dev‰" dataDxfId="48">
+      <calculatedColumnFormula>ABS(M2-I2)*1000</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="A1:G26" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:G26"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="0" dataDxfId="23"/>
+    <tableColumn id="2" name="1" dataDxfId="22"/>
+    <tableColumn id="3" name="2" dataDxfId="21"/>
+    <tableColumn id="4" name="3" dataDxfId="20"/>
+    <tableColumn id="5" name="4" dataDxfId="19"/>
+    <tableColumn id="6" name="5" dataDxfId="18"/>
+    <tableColumn id="7" name="6" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="I10:J11" totalsRowShown="0">
+  <autoFilter ref="I10:J11"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="a" dataDxfId="13"/>
+    <tableColumn id="2" name="b" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Målinger" displayName="Målinger" ref="A1:G26" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:G26"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="0" dataDxfId="11"/>
+    <tableColumn id="2" name="1" dataDxfId="10"/>
+    <tableColumn id="3" name="2" dataDxfId="9"/>
+    <tableColumn id="4" name="3" dataDxfId="8"/>
+    <tableColumn id="5" name="4" dataDxfId="7"/>
+    <tableColumn id="6" name="5" dataDxfId="6"/>
+    <tableColumn id="7" name="6" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="M1:N8" totalsRowShown="0">
+  <autoFilter ref="M1:N8"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="px2mm" dataDxfId="55">
+      <calculatedColumnFormula>(J2-$J$11)/$I$11</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="dev‰" dataDxfId="54">
+      <calculatedColumnFormula>ABS(M2-I2)*1000</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="I1:K8" totalsRowShown="0">
+  <autoFilter ref="I1:K8"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="mm"/>
+    <tableColumn id="2" name="avg" dataDxfId="53"/>
+    <tableColumn id="3" name="stddev" dataDxfId="52"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="I10:J11" totalsRowShown="0">
+  <autoFilter ref="I10:J11"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="a" dataDxfId="15"/>
+    <tableColumn id="2" name="b" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table27911" displayName="Table27911" ref="M1:N8" totalsRowShown="0">
+  <autoFilter ref="M1:N8"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="px2mm" dataDxfId="41">
+      <calculatedColumnFormula>(J2-$J$11)/$I$11</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="dev‰" dataDxfId="40">
+      <calculatedColumnFormula>ABS(M2-I2)*1000</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:G51" totalsRowShown="0" headerRowDxfId="32">
+  <autoFilter ref="A1:G51"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="0" dataDxfId="39"/>
+    <tableColumn id="2" name="1" dataDxfId="38"/>
+    <tableColumn id="3" name="2" dataDxfId="37"/>
+    <tableColumn id="4" name="3" dataDxfId="36"/>
+    <tableColumn id="5" name="4" dataDxfId="35"/>
+    <tableColumn id="6" name="5" dataDxfId="34"/>
+    <tableColumn id="7" name="6" dataDxfId="33"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="I10:J11" totalsRowShown="0">
+  <autoFilter ref="I10:J11"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="a" dataDxfId="1"/>
+    <tableColumn id="2" name="b" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table368" displayName="Table368" ref="I1:K8" totalsRowShown="0">
+  <autoFilter ref="I1:K8"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="mm"/>
+    <tableColumn id="2" name="avg" dataDxfId="47"/>
+    <tableColumn id="3" name="stddev" dataDxfId="46"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table279" displayName="Table279" ref="M1:N8" totalsRowShown="0">
   <autoFilter ref="M1:N8"/>
   <tableColumns count="2">
     <tableColumn id="1" name="px2mm" dataDxfId="45">
@@ -7351,167 +7513,17 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="A1:G26" totalsRowShown="0" headerRowDxfId="12">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A1:G26" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A1:G26"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="0" dataDxfId="19"/>
-    <tableColumn id="2" name="1" dataDxfId="18"/>
-    <tableColumn id="3" name="2" dataDxfId="17"/>
-    <tableColumn id="4" name="3" dataDxfId="16"/>
-    <tableColumn id="5" name="4" dataDxfId="15"/>
-    <tableColumn id="6" name="5" dataDxfId="14"/>
-    <tableColumn id="7" name="6" dataDxfId="13"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="I10:J11" totalsRowShown="0">
-  <autoFilter ref="I10:J11"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="a" dataDxfId="9"/>
-    <tableColumn id="2" name="b" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Målinger" displayName="Målinger" ref="A1:G26" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:G26"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="0" dataDxfId="7"/>
-    <tableColumn id="2" name="1" dataDxfId="6"/>
-    <tableColumn id="3" name="2" dataDxfId="5"/>
-    <tableColumn id="4" name="3" dataDxfId="4"/>
-    <tableColumn id="5" name="4" dataDxfId="3"/>
-    <tableColumn id="6" name="5" dataDxfId="2"/>
-    <tableColumn id="7" name="6" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="M1:N8" totalsRowShown="0">
-  <autoFilter ref="M1:N8"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="px2mm" dataDxfId="51">
-      <calculatedColumnFormula>(J2-$J$11)/$I$11</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" name="dev‰" dataDxfId="50">
-      <calculatedColumnFormula>ABS(M2-I2)*1000</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="I1:K8" totalsRowShown="0">
-  <autoFilter ref="I1:K8"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="mm"/>
-    <tableColumn id="2" name="avg" dataDxfId="49"/>
-    <tableColumn id="3" name="stddev" dataDxfId="48"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="I10:J11" totalsRowShown="0">
-  <autoFilter ref="I10:J11"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="a" dataDxfId="11"/>
-    <tableColumn id="2" name="b" dataDxfId="10"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table27911" displayName="Table27911" ref="M1:N8" totalsRowShown="0">
-  <autoFilter ref="M1:N8"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="px2mm" dataDxfId="37">
-      <calculatedColumnFormula>(J2-$J$11)/$I$11</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" name="dev‰" dataDxfId="36">
-      <calculatedColumnFormula>ABS(M2-I2)*1000</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:G51" totalsRowShown="0" headerRowDxfId="28">
-  <autoFilter ref="A1:G51"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="0" dataDxfId="35"/>
-    <tableColumn id="2" name="1" dataDxfId="34"/>
-    <tableColumn id="3" name="2" dataDxfId="33"/>
-    <tableColumn id="4" name="3" dataDxfId="32"/>
-    <tableColumn id="5" name="4" dataDxfId="31"/>
-    <tableColumn id="6" name="5" dataDxfId="30"/>
-    <tableColumn id="7" name="6" dataDxfId="29"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="I10:J11" totalsRowShown="0">
-  <autoFilter ref="I10:J11"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="a"/>
-    <tableColumn id="2" name="b"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table368" displayName="Table368" ref="I1:K8" totalsRowShown="0">
-  <autoFilter ref="I1:K8"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="mm"/>
-    <tableColumn id="2" name="avg" dataDxfId="43"/>
-    <tableColumn id="3" name="stddev" dataDxfId="42"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table279" displayName="Table279" ref="M1:N8" totalsRowShown="0">
-  <autoFilter ref="M1:N8"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="px2mm" dataDxfId="41">
-      <calculatedColumnFormula>(J2-$J$11)/$I$11</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" name="dev‰" dataDxfId="40">
-      <calculatedColumnFormula>ABS(M2-I2)*1000</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A1:G26" totalsRowShown="0" headerRowDxfId="20">
-  <autoFilter ref="A1:G26"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="0" dataDxfId="27"/>
-    <tableColumn id="2" name="1" dataDxfId="26"/>
-    <tableColumn id="3" name="2" dataDxfId="25"/>
-    <tableColumn id="4" name="3" dataDxfId="24"/>
-    <tableColumn id="5" name="4" dataDxfId="23"/>
-    <tableColumn id="6" name="5" dataDxfId="22"/>
-    <tableColumn id="7" name="6" dataDxfId="21"/>
+    <tableColumn id="1" name="0" dataDxfId="31"/>
+    <tableColumn id="2" name="1" dataDxfId="30"/>
+    <tableColumn id="3" name="2" dataDxfId="29"/>
+    <tableColumn id="4" name="3" dataDxfId="28"/>
+    <tableColumn id="5" name="4" dataDxfId="27"/>
+    <tableColumn id="6" name="5" dataDxfId="26"/>
+    <tableColumn id="7" name="6" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7521,8 +7533,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="I10:J11" totalsRowShown="0">
   <autoFilter ref="I10:J11"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="a"/>
-    <tableColumn id="2" name="b"/>
+    <tableColumn id="1" name="a" dataDxfId="2"/>
+    <tableColumn id="2" name="b" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7533,8 +7545,8 @@
   <autoFilter ref="I1:K8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="mm"/>
-    <tableColumn id="2" name="avg" dataDxfId="47"/>
-    <tableColumn id="3" name="stddev" dataDxfId="46"/>
+    <tableColumn id="2" name="avg" dataDxfId="51"/>
+    <tableColumn id="3" name="stddev" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7843,7 +7855,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8258,10 +8270,10 @@
       <c r="G11" s="1">
         <v>45.210921999999997</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>7.1924332778571403</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>1.7451563521428499</v>
       </c>
     </row>
@@ -9227,7 +9239,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I11" activeCellId="1" sqref="J11 I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9642,10 +9654,10 @@
       <c r="G11" s="1">
         <v>45.446615999999999</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>7.3040976400000002</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="1">
         <v>1.41051214857144</v>
       </c>
     </row>
@@ -10841,7 +10853,9 @@
   </sheetPr>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
update + new measurement base = 0.98mm instead of 1.00mm
</commit_message>
<xml_diff>
--- a/testOpenCV/tg_r2.xlsx
+++ b/testOpenCV/tg_r2.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
   <si>
     <t>4</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>dev‰</t>
+  </si>
+  <si>
+    <t>Enhed</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="57">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -187,12 +214,6 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -253,22 +274,7 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -464,22 +470,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>1.96</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2.94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3.92</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>5.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4195,8 +4201,8 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1560171" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -4238,6 +4244,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4254,13 +4261,7 @@
                       <a:rPr lang="da-DK" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=7,46</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="da-DK" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>689414857143 </m:t>
+                      <m:t>=7,46689414857143 </m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -4270,7 +4271,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -4346,8 +4347,8 @@
       <xdr:rowOff>17938</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1573251" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -4389,6 +4390,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4405,13 +4407,7 @@
                       <a:rPr lang="da-DK" sz="1100" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="da-DK" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>0,705060611428582</m:t>
+                      <m:t>=0,705060611428582</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -4421,7 +4417,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -4497,8 +4493,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2062038" cy="337593"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -4540,6 +4536,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4630,6 +4627,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4650,7 +4648,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -4757,8 +4755,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1239827" cy="320280"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -4800,6 +4798,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -4875,7 +4874,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -4982,8 +4981,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1007392" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -5025,6 +5024,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -5066,7 +5066,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -5157,8 +5157,8 @@
       <xdr:rowOff>8413</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1473865" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -5200,6 +5200,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -5235,7 +5236,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -5325,8 +5326,8 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2062038" cy="337593"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -5368,6 +5369,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -5458,6 +5460,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -5478,7 +5481,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -5585,8 +5588,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1239827" cy="320280"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -5628,6 +5631,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -5703,7 +5707,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -5810,8 +5814,8 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1560171" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -5853,6 +5857,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -5869,13 +5874,7 @@
                       <a:rPr lang="da-DK" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=7,46</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="da-DK" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>689414857143 </m:t>
+                      <m:t>=7,46689414857143 </m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -5885,7 +5884,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -5961,8 +5960,8 @@
       <xdr:rowOff>8413</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1573251" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -6004,6 +6003,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6020,13 +6020,7 @@
                       <a:rPr lang="da-DK" sz="1100" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="da-DK" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>0,705060611428582</m:t>
+                      <m:t>=0,705060611428582</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -6036,7 +6030,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -6112,8 +6106,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2062038" cy="337593"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -6155,6 +6149,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6245,6 +6240,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6265,7 +6261,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -6372,8 +6368,8 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1239827" cy="320280"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -6415,6 +6411,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6490,7 +6487,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8">
@@ -6597,8 +6594,8 @@
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1560171" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -6640,6 +6637,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6656,13 +6654,7 @@
                       <a:rPr lang="da-DK" sz="1100" b="0" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=7,60</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="da-DK" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>628964714286 </m:t>
+                      <m:t>=7,60628964714286 </m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -6672,7 +6664,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -6748,8 +6740,8 @@
       <xdr:rowOff>94138</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1495153" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -6791,6 +6783,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -6807,13 +6800,7 @@
                       <a:rPr lang="da-DK" sz="1100" i="1">
                         <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="da-DK" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>1,89343821285715</m:t>
+                      <m:t>=1,89343821285715</m:t>
                     </m:r>
                   </m:oMath>
                 </m:oMathPara>
@@ -6823,7 +6810,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -6899,8 +6886,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2062038" cy="337593"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -6942,6 +6929,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -7032,6 +7020,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -7052,7 +7041,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -7159,8 +7148,8 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1239827" cy="320280"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -7202,6 +7191,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -7277,7 +7267,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -7341,8 +7331,8 @@
   <autoFilter ref="I1:K8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="mm"/>
-    <tableColumn id="2" name="avg" dataDxfId="43"/>
-    <tableColumn id="3" name="stddev" dataDxfId="42"/>
+    <tableColumn id="2" name="avg" dataDxfId="56"/>
+    <tableColumn id="3" name="stddev" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7352,10 +7342,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="M1:N8" totalsRowShown="0">
   <autoFilter ref="M1:N8"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="px2mm" dataDxfId="49">
+    <tableColumn id="1" name="px2mm" dataDxfId="26">
       <calculatedColumnFormula>(J2-$J$11)/$I$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="dev‰" dataDxfId="48">
+    <tableColumn id="2" name="dev‰" dataDxfId="25">
       <calculatedColumnFormula>ABS(M2-I2)*1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7364,7 +7354,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="A1:G26" totalsRowShown="0" headerRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="A1:G26" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A1:G26"/>
   <tableColumns count="7">
     <tableColumn id="1" name="0" dataDxfId="23"/>
@@ -7383,24 +7373,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table16" displayName="Table16" ref="I10:J11" totalsRowShown="0">
   <autoFilter ref="I10:J11"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="a" dataDxfId="13"/>
-    <tableColumn id="2" name="b" dataDxfId="12"/>
+    <tableColumn id="1" name="a" dataDxfId="16"/>
+    <tableColumn id="2" name="b" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Målinger" displayName="Målinger" ref="A1:G26" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Målinger" displayName="Målinger" ref="A1:G26" totalsRowShown="0" dataDxfId="14">
   <autoFilter ref="A1:G26"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="0" dataDxfId="11"/>
-    <tableColumn id="2" name="1" dataDxfId="10"/>
-    <tableColumn id="3" name="2" dataDxfId="9"/>
-    <tableColumn id="4" name="3" dataDxfId="8"/>
-    <tableColumn id="5" name="4" dataDxfId="7"/>
-    <tableColumn id="6" name="5" dataDxfId="6"/>
-    <tableColumn id="7" name="6" dataDxfId="5"/>
+    <tableColumn id="1" name="0" dataDxfId="13"/>
+    <tableColumn id="2" name="1" dataDxfId="12"/>
+    <tableColumn id="3" name="2" dataDxfId="11"/>
+    <tableColumn id="4" name="3" dataDxfId="10"/>
+    <tableColumn id="5" name="4" dataDxfId="9"/>
+    <tableColumn id="6" name="5" dataDxfId="8"/>
+    <tableColumn id="7" name="6" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7410,10 +7400,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="M1:N8" totalsRowShown="0">
   <autoFilter ref="M1:N8"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="px2mm" dataDxfId="55">
+    <tableColumn id="1" name="px2mm" dataDxfId="6">
       <calculatedColumnFormula>(J2-$J$11)/$I$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="dev‰" dataDxfId="54">
+    <tableColumn id="2" name="dev‰" dataDxfId="5">
       <calculatedColumnFormula>ABS(M2-I2)*1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7426,8 +7416,8 @@
   <autoFilter ref="I1:K8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="mm"/>
-    <tableColumn id="2" name="avg" dataDxfId="53"/>
-    <tableColumn id="3" name="stddev" dataDxfId="52"/>
+    <tableColumn id="2" name="avg" dataDxfId="4"/>
+    <tableColumn id="3" name="stddev" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7437,8 +7427,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table17" displayName="Table17" ref="I10:J11" totalsRowShown="0">
   <autoFilter ref="I10:J11"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="a" dataDxfId="15"/>
-    <tableColumn id="2" name="b" dataDxfId="14"/>
+    <tableColumn id="1" name="a" dataDxfId="2"/>
+    <tableColumn id="2" name="b" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7448,10 +7438,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table27911" displayName="Table27911" ref="M1:N8" totalsRowShown="0">
   <autoFilter ref="M1:N8"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="px2mm" dataDxfId="41">
+    <tableColumn id="1" name="px2mm" dataDxfId="54">
       <calculatedColumnFormula>(J2-$J$11)/$I$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="dev‰" dataDxfId="40">
+    <tableColumn id="2" name="dev‰" dataDxfId="53">
       <calculatedColumnFormula>ABS(M2-I2)*1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7460,16 +7450,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:G51" totalsRowShown="0" headerRowDxfId="32">
-  <autoFilter ref="A1:G51"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="0" dataDxfId="39"/>
-    <tableColumn id="2" name="1" dataDxfId="38"/>
-    <tableColumn id="3" name="2" dataDxfId="37"/>
-    <tableColumn id="4" name="3" dataDxfId="36"/>
-    <tableColumn id="5" name="4" dataDxfId="35"/>
-    <tableColumn id="6" name="5" dataDxfId="34"/>
-    <tableColumn id="7" name="6" dataDxfId="33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:H51" totalsRowShown="0" headerRowDxfId="52">
+  <autoFilter ref="A1:H51"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="0" dataDxfId="51"/>
+    <tableColumn id="2" name="1" dataDxfId="50"/>
+    <tableColumn id="3" name="2" dataDxfId="49"/>
+    <tableColumn id="4" name="3" dataDxfId="48"/>
+    <tableColumn id="5" name="4" dataDxfId="47"/>
+    <tableColumn id="6" name="5" dataDxfId="46"/>
+    <tableColumn id="7" name="6" dataDxfId="45"/>
+    <tableColumn id="8" name="Enhed" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7479,8 +7470,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="I10:J11" totalsRowShown="0">
   <autoFilter ref="I10:J11"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="a" dataDxfId="1"/>
-    <tableColumn id="2" name="b" dataDxfId="0"/>
+    <tableColumn id="1" name="a" dataDxfId="44"/>
+    <tableColumn id="2" name="b" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7491,8 +7482,8 @@
   <autoFilter ref="I1:K8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="mm"/>
-    <tableColumn id="2" name="avg" dataDxfId="47"/>
-    <tableColumn id="3" name="stddev" dataDxfId="46"/>
+    <tableColumn id="2" name="avg" dataDxfId="42"/>
+    <tableColumn id="3" name="stddev" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7502,10 +7493,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table279" displayName="Table279" ref="M1:N8" totalsRowShown="0">
   <autoFilter ref="M1:N8"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="px2mm" dataDxfId="45">
+    <tableColumn id="1" name="px2mm" dataDxfId="40">
       <calculatedColumnFormula>(J2-$J$11)/$I$11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="dev‰" dataDxfId="44">
+    <tableColumn id="2" name="dev‰" dataDxfId="39">
       <calculatedColumnFormula>ABS(M2-I2)*1000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7514,16 +7505,16 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A1:G26" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="A1:G26" totalsRowShown="0" headerRowDxfId="38">
   <autoFilter ref="A1:G26"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="0" dataDxfId="31"/>
-    <tableColumn id="2" name="1" dataDxfId="30"/>
-    <tableColumn id="3" name="2" dataDxfId="29"/>
-    <tableColumn id="4" name="3" dataDxfId="28"/>
-    <tableColumn id="5" name="4" dataDxfId="27"/>
-    <tableColumn id="6" name="5" dataDxfId="26"/>
-    <tableColumn id="7" name="6" dataDxfId="25"/>
+    <tableColumn id="1" name="0" dataDxfId="37"/>
+    <tableColumn id="2" name="1" dataDxfId="36"/>
+    <tableColumn id="3" name="2" dataDxfId="35"/>
+    <tableColumn id="4" name="3" dataDxfId="34"/>
+    <tableColumn id="5" name="4" dataDxfId="33"/>
+    <tableColumn id="6" name="5" dataDxfId="32"/>
+    <tableColumn id="7" name="6" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7533,8 +7524,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="I10:J11" totalsRowShown="0">
   <autoFilter ref="I10:J11"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="a" dataDxfId="2"/>
-    <tableColumn id="2" name="b" dataDxfId="3"/>
+    <tableColumn id="1" name="a" dataDxfId="30"/>
+    <tableColumn id="2" name="b" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7545,8 +7536,8 @@
   <autoFilter ref="I1:K8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="mm"/>
-    <tableColumn id="2" name="avg" dataDxfId="51"/>
-    <tableColumn id="3" name="stddev" dataDxfId="50"/>
+    <tableColumn id="2" name="avg" dataDxfId="28"/>
+    <tableColumn id="3" name="stddev" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7855,7 +7846,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7886,6 +7877,9 @@
       <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="I1" t="s">
         <v>1</v>
       </c>
@@ -7924,6 +7918,9 @@
       <c r="G2" s="1">
         <v>45.487141000000001</v>
       </c>
+      <c r="H2" s="1">
+        <v>0.98</v>
+      </c>
       <c r="I2">
         <v>0</v>
       </c>
@@ -7936,7 +7933,7 @@
         <v>0.68003707355587895</v>
       </c>
       <c r="M2" s="1">
-        <f>(J2-$J$11)/$I$11</f>
+        <f t="shared" ref="M2:M8" si="0">(J2-$J$11)/$I$11</f>
         <v>0.16847709266733335</v>
       </c>
       <c r="N2" s="1">
@@ -7966,8 +7963,10 @@
       <c r="G3" s="1">
         <v>45.606758999999997</v>
       </c>
+      <c r="H3" s="1"/>
       <c r="I3">
-        <v>1</v>
+        <f>1*$H$2</f>
+        <v>0.98</v>
       </c>
       <c r="J3" s="1">
         <f>AVERAGE(B2:B51)</f>
@@ -7978,12 +7977,12 @@
         <v>0.13256666257583152</v>
       </c>
       <c r="M3" s="1">
-        <f>(J3-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>0.89495537312442275</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N8" si="0">ABS(M3-I3)*1000</f>
-        <v>105.04462687557725</v>
+        <f t="shared" ref="N3:N8" si="1">ABS(M3-I3)*1000</f>
+        <v>85.044626875577237</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -8008,8 +8007,10 @@
       <c r="G4" s="1">
         <v>45.473323000000001</v>
       </c>
+      <c r="H4" s="1"/>
       <c r="I4">
-        <v>2</v>
+        <f>2*$H$2</f>
+        <v>1.96</v>
       </c>
       <c r="J4" s="1">
         <f>AVERAGE(C2:C51)</f>
@@ -8020,12 +8021,12 @@
         <v>8.9007974635768414E-2</v>
       </c>
       <c r="M4" s="1">
-        <f>(J4-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>1.9445132220988732</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="0"/>
-        <v>55.486777901126771</v>
+        <f t="shared" si="1"/>
+        <v>15.486777901126736</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -8050,8 +8051,10 @@
       <c r="G5" s="1">
         <v>45.004337999999997</v>
       </c>
+      <c r="H5" s="1"/>
       <c r="I5">
-        <v>3</v>
+        <f>3*$H$2</f>
+        <v>2.94</v>
       </c>
       <c r="J5" s="1">
         <f>AVERAGE(D2:D51)</f>
@@ -8062,12 +8065,12 @@
         <v>0.41057380987455289</v>
       </c>
       <c r="M5" s="1">
-        <f>(J5-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>2.9192334105479056</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="0"/>
-        <v>80.766589452094365</v>
+        <f t="shared" si="1"/>
+        <v>20.766589452094308</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -8092,8 +8095,10 @@
       <c r="G6" s="1">
         <v>45.668478999999998</v>
       </c>
+      <c r="H6" s="1"/>
       <c r="I6">
-        <v>4</v>
+        <f>4*$H$2</f>
+        <v>3.92</v>
       </c>
       <c r="J6" s="1">
         <f>AVERAGE(E2:E51)</f>
@@ -8104,12 +8109,12 @@
         <v>0.11848661513473313</v>
       </c>
       <c r="M6" s="1">
-        <f>(J6-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>3.9906027764234535</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="0"/>
-        <v>9.3972235765464873</v>
+        <f t="shared" si="1"/>
+        <v>70.602776423453577</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -8134,8 +8139,10 @@
       <c r="G7" s="1">
         <v>45.671895999999997</v>
       </c>
+      <c r="H7" s="1"/>
       <c r="I7">
-        <v>5</v>
+        <f>5*$H$2</f>
+        <v>4.9000000000000004</v>
       </c>
       <c r="J7" s="1">
         <f>AVERAGE(F2:F51)</f>
@@ -8146,12 +8153,12 @@
         <v>0.12942977282953694</v>
       </c>
       <c r="M7" s="1">
-        <f>(J7-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>4.9974019054878029</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="0"/>
-        <v>2.5980945121970578</v>
+        <f t="shared" si="1"/>
+        <v>97.401905487802594</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -8176,8 +8183,10 @@
       <c r="G8" s="1">
         <v>45.561048999999997</v>
       </c>
+      <c r="H8" s="1"/>
       <c r="I8">
-        <v>6</v>
+        <f>6*$H$2</f>
+        <v>5.88</v>
       </c>
       <c r="J8" s="1">
         <f>AVERAGE(G2:G51)</f>
@@ -8188,12 +8197,12 @@
         <v>0.12887268826209733</v>
       </c>
       <c r="M8" s="1">
-        <f>(J8-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>6.0848162196502233</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="0"/>
-        <v>84.816219650223346</v>
+        <f t="shared" si="1"/>
+        <v>204.81621965022345</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -8218,6 +8227,7 @@
       <c r="G9" s="1">
         <v>45.626207000000001</v>
       </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -8241,6 +8251,7 @@
       <c r="G10" s="1">
         <v>45.564689000000001</v>
       </c>
+      <c r="H10" s="1"/>
       <c r="I10" t="s">
         <v>5</v>
       </c>
@@ -8270,6 +8281,7 @@
       <c r="G11" s="1">
         <v>45.210921999999997</v>
       </c>
+      <c r="H11" s="1"/>
       <c r="I11" s="1">
         <v>7.1924332778571403</v>
       </c>
@@ -8299,6 +8311,7 @@
       <c r="G12" s="1">
         <v>45.570596000000002</v>
       </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -8322,6 +8335,7 @@
       <c r="G13" s="1">
         <v>45.746613000000004</v>
       </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -8345,6 +8359,7 @@
       <c r="G14" s="1">
         <v>45.496529000000002</v>
       </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -8368,6 +8383,7 @@
       <c r="G15" s="1">
         <v>45.542391000000002</v>
       </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -8391,8 +8407,9 @@
       <c r="G16" s="1">
         <v>45.521802000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2.8740800000000002</v>
       </c>
@@ -8414,8 +8431,9 @@
       <c r="G17" s="1">
         <v>45.455635999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2.8660299999999999</v>
       </c>
@@ -8437,8 +8455,9 @@
       <c r="G18" s="1">
         <v>45.324975999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1.8220799999999999</v>
       </c>
@@ -8460,8 +8479,9 @@
       <c r="G19" s="1">
         <v>45.488613999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1.94232</v>
       </c>
@@ -8483,8 +8503,9 @@
       <c r="G20" s="1">
         <v>45.537799999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3.6547900000000002</v>
       </c>
@@ -8506,8 +8527,9 @@
       <c r="G21" s="1">
         <v>45.575493999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>3.2837499999999999</v>
       </c>
@@ -8529,8 +8551,9 @@
       <c r="G22" s="1">
         <v>45.578932000000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2.8456399999999999</v>
       </c>
@@ -8552,8 +8575,9 @@
       <c r="G23" s="1">
         <v>45.597287000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>3.2759399999999999</v>
       </c>
@@ -8575,8 +8599,9 @@
       <c r="G24" s="1">
         <v>45.374195999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1.94452</v>
       </c>
@@ -8598,8 +8623,9 @@
       <c r="G25" s="1">
         <v>45.599074999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1.9436599999999999</v>
       </c>
@@ -8621,8 +8647,9 @@
       <c r="G26" s="1">
         <v>45.494526999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>3.20825</v>
       </c>
@@ -8644,8 +8671,9 @@
       <c r="G27" s="1">
         <v>45.647556999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>3.2975500000000002</v>
       </c>
@@ -8667,8 +8695,9 @@
       <c r="G28" s="1">
         <v>45.512618000000003</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>3.26227</v>
       </c>
@@ -8690,8 +8719,9 @@
       <c r="G29" s="1">
         <v>45.256993000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>3.3375900000000001</v>
       </c>
@@ -8713,8 +8743,9 @@
       <c r="G30" s="1">
         <v>45.668573000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>3.3317299999999999</v>
       </c>
@@ -8736,8 +8767,9 @@
       <c r="G31" s="1">
         <v>45.638264999999997</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>3.3729200000000001</v>
       </c>
@@ -8759,8 +8791,9 @@
       <c r="G32" s="1">
         <v>45.324365</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>3.4813800000000001</v>
       </c>
@@ -8782,8 +8815,9 @@
       <c r="G33" s="1">
         <v>45.412962999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>3.9319500000000001</v>
       </c>
@@ -8805,8 +8839,9 @@
       <c r="G34" s="1">
         <v>45.290559999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1.17804</v>
       </c>
@@ -8828,8 +8863,9 @@
       <c r="G35" s="1">
         <v>45.526136999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2.8797000000000001</v>
       </c>
@@ -8851,8 +8887,9 @@
       <c r="G36" s="1">
         <v>45.582956000000003</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>1.6771199999999999</v>
       </c>
@@ -8874,8 +8911,9 @@
       <c r="G37" s="1">
         <v>45.575797999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>3.3087800000000001</v>
       </c>
@@ -8897,8 +8935,9 @@
       <c r="G38" s="1">
         <v>45.479804999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>3.4368300000000001</v>
       </c>
@@ -8920,8 +8959,9 @@
       <c r="G39" s="1">
         <v>45.475346000000002</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>1.9567300000000001</v>
       </c>
@@ -8943,8 +8983,9 @@
       <c r="G40" s="1">
         <v>45.568007000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2.69</v>
       </c>
@@ -8966,8 +9007,9 @@
       <c r="G41" s="1">
         <v>45.551453000000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>4.0155000000000003</v>
       </c>
@@ -8989,8 +9031,9 @@
       <c r="G42" s="1">
         <v>45.525787999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>3.31915</v>
       </c>
@@ -9012,8 +9055,9 @@
       <c r="G43" s="1">
         <v>45.527360999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>4.0354000000000001</v>
       </c>
@@ -9035,8 +9079,9 @@
       <c r="G44" s="1">
         <v>45.523848000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2.7863799999999999</v>
       </c>
@@ -9058,8 +9103,9 @@
       <c r="G45" s="1">
         <v>45.410842000000002</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>3.3969100000000001</v>
       </c>
@@ -9081,8 +9127,9 @@
       <c r="G46" s="1">
         <v>45.536431999999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>3.3514400000000002</v>
       </c>
@@ -9104,8 +9151,9 @@
       <c r="G47" s="1">
         <v>45.567779999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>3.4115600000000001</v>
       </c>
@@ -9127,6 +9175,7 @@
       <c r="G48" s="1">
         <v>45.595643000000003</v>
       </c>
+      <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
@@ -9150,6 +9199,7 @@
       <c r="G49" s="1">
         <v>45.471992999999998</v>
       </c>
+      <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
@@ -9173,6 +9223,7 @@
       <c r="G50" s="1">
         <v>45.476962</v>
       </c>
+      <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
@@ -9196,6 +9247,7 @@
       <c r="G51" s="1">
         <v>45.562235000000001</v>
       </c>
+      <c r="H51" s="1"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J55" s="1"/>
@@ -9320,7 +9372,7 @@
         <v>0.84605409508115392</v>
       </c>
       <c r="M2" s="1">
-        <f>(J2-$J$11)/$I$11</f>
+        <f t="shared" ref="M2:M8" si="0">(J2-$J$11)/$I$11</f>
         <v>0.11065599766935209</v>
       </c>
       <c r="N2" s="1">
@@ -9362,11 +9414,11 @@
         <v>5.4647066976136929E-2</v>
       </c>
       <c r="M3" s="1">
-        <f>(J3-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>0.93191890729277838</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N8" si="0">ABS(M3-I3)*1000</f>
+        <f t="shared" ref="N3:N8" si="1">ABS(M3-I3)*1000</f>
         <v>68.081092707221629</v>
       </c>
     </row>
@@ -9404,11 +9456,11 @@
         <v>0.10385946570148712</v>
       </c>
       <c r="M4" s="1">
-        <f>(J4-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>1.9571397475771641</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42.860252422835863</v>
       </c>
     </row>
@@ -9446,11 +9498,11 @@
         <v>0.14243056179767019</v>
       </c>
       <c r="M5" s="1">
-        <f>(J5-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>2.9607853450640023</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39.214654935997743</v>
       </c>
     </row>
@@ -9488,11 +9540,11 @@
         <v>0.10819041971728212</v>
       </c>
       <c r="M6" s="1">
-        <f>(J6-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>3.9808582202124776</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.141779787522406</v>
       </c>
     </row>
@@ -9530,11 +9582,11 @@
         <v>0.16577083497505382</v>
       </c>
       <c r="M7" s="1">
-        <f>(J7-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>5.0038380115943468</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.838011594346824</v>
       </c>
     </row>
@@ -9572,11 +9624,11 @@
         <v>0.18306303123436335</v>
       </c>
       <c r="M8" s="1">
-        <f>(J8-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>6.0548037705898681</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.803770589868073</v>
       </c>
     </row>
@@ -10144,7 +10196,7 @@
         <v>1.5515003707431071E-2</v>
       </c>
       <c r="M2" s="1">
-        <f>(J2-$J$11)/$I$11</f>
+        <f t="shared" ref="M2:M8" si="0">(J2-$J$11)/$I$11</f>
         <v>-7.6877096612926491E-4</v>
       </c>
       <c r="N2" s="1">
@@ -10186,11 +10238,11 @@
         <v>5.4647066976136929E-2</v>
       </c>
       <c r="M3" s="1">
-        <f>(J3-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>1.0060780398244527</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N8" si="0">ABS(M3-I3)*1000</f>
+        <f t="shared" ref="N3:N8" si="1">ABS(M3-I3)*1000</f>
         <v>6.0780398244526523</v>
       </c>
     </row>
@@ -10228,11 +10280,11 @@
         <v>0.10385946570148712</v>
       </c>
       <c r="M4" s="1">
-        <f>(J4-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>2.0089465646759357</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.9465646759356865</v>
       </c>
     </row>
@@ -10270,11 +10322,11 @@
         <v>0.14243056179767019</v>
       </c>
       <c r="M5" s="1">
-        <f>(J5-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>2.9907102396575236</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.2897603424764164</v>
       </c>
     </row>
@@ -10312,11 +10364,11 @@
         <v>0.10819041971728212</v>
       </c>
       <c r="M6" s="1">
-        <f>(J6-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>3.9885430375719637</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.456962428036288</v>
       </c>
     </row>
@@ -10354,11 +10406,11 @@
         <v>0.16577083497505382</v>
       </c>
       <c r="M7" s="1">
-        <f>(J7-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>4.9892193738542367</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.78062614576325</v>
       </c>
     </row>
@@ -10396,11 +10448,11 @@
         <v>0.18306303123436335</v>
       </c>
       <c r="M8" s="1">
-        <f>(J8-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>6.0172715153820029</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.271515382002889</v>
       </c>
     </row>
@@ -10934,7 +10986,7 @@
         <v>0.25207450750553984</v>
       </c>
       <c r="M2" s="1">
-        <f>(J2-$J$11)/$I$11</f>
+        <f t="shared" ref="M2:M8" si="0">(J2-$J$11)/$I$11</f>
         <v>-1.3220429081993086E-2</v>
       </c>
       <c r="N2" s="1">
@@ -10976,11 +11028,11 @@
         <v>0.21738084451450626</v>
       </c>
       <c r="M3" s="1">
-        <f>(J3-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>1.0344017059747759</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N8" si="0">ABS(M3-I3)*1000</f>
+        <f t="shared" ref="N3:N8" si="1">ABS(M3-I3)*1000</f>
         <v>34.401705974775879</v>
       </c>
     </row>
@@ -11018,11 +11070,11 @@
         <v>0.45650594060929234</v>
       </c>
       <c r="M4" s="1">
-        <f>(J4-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>2.0019771338661521</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9771338661520588</v>
       </c>
     </row>
@@ -11060,11 +11112,11 @@
         <v>0.1918651136196925</v>
       </c>
       <c r="M5" s="1">
-        <f>(J5-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>2.9823305658184847</v>
       </c>
       <c r="N5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.669434181515342</v>
       </c>
     </row>
@@ -11102,11 +11154,11 @@
         <v>0.18017463405501191</v>
       </c>
       <c r="M6" s="1">
-        <f>(J6-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>3.9713590342289393</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28.640965771060678</v>
       </c>
     </row>
@@ -11144,11 +11196,11 @@
         <v>4.9209310460457047E-2</v>
       </c>
       <c r="M7" s="1">
-        <f>(J7-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>5.0096957432401039</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.6957432401039156</v>
       </c>
     </row>
@@ -11186,11 +11238,11 @@
         <v>0.13829212922852829</v>
       </c>
       <c r="M8" s="1">
-        <f>(J8-$J$11)/$I$11</f>
+        <f t="shared" si="0"/>
         <v>6.0134562459535239</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.456245953523904</v>
       </c>
     </row>

</xml_diff>